<commit_message>
Integre el registro de proyectos tanto individual como masivos
</commit_message>
<xml_diff>
--- a/src/assets/docs/registro_proyectos.xlsx
+++ b/src/assets/docs/registro_proyectos.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nombre</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Nombre del Coordinador</t>
+  </si>
+  <si>
+    <t>Correo del Coordinador</t>
+  </si>
+  <si>
+    <t>Teléfono del Coordinador</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,9 +426,11 @@
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" customWidth="1"/>
     <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,6 +453,12 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modifique el excel de proyectos
</commit_message>
<xml_diff>
--- a/src/assets/docs/registro_proyectos.xlsx
+++ b/src/assets/docs/registro_proyectos.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Nombre</t>
   </si>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,10 +427,11 @@
     <col min="7" max="7" width="24.5703125" customWidth="1"/>
     <col min="8" max="8" width="23.42578125" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,6 +461,9 @@
       </c>
       <c r="J1" t="s">
         <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>